<commit_message>
Finished the project. Perhaps continue in future.
</commit_message>
<xml_diff>
--- a/GAN Results/GAN Results.xlsx
+++ b/GAN Results/GAN Results.xlsx
@@ -600,14 +600,14 @@
   <dimension ref="A1:AF61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.33203125" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.109375" bestFit="1" customWidth="1"/>

</xml_diff>